<commit_message>
Annotated WT clusters in Seurat
</commit_message>
<xml_diff>
--- a/st_clusters_fusca.xlsx
+++ b/st_clusters_fusca.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patron\Documents\MyDocuments\R\CAR-T\CAR-T-subpopulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E43DB283-8AB7-4605-9D0F-6954D4E93C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB78A715-83D4-4741-903F-814A1CFB7993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="st_clusters_fusca" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3309" uniqueCount="3290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3318" uniqueCount="3293">
   <si>
     <t>population</t>
   </si>
@@ -9891,12 +9891,21 @@
   </si>
   <si>
     <t>Regulatory T</t>
+  </si>
+  <si>
+    <t>HLA-DP</t>
+  </si>
+  <si>
+    <t>HLA-DM</t>
+  </si>
+  <si>
+    <t>Dendritic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -10732,11 +10741,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3261"/>
   <sheetViews>
-    <sheetView topLeftCell="A3242" workbookViewId="0">
-      <selection activeCell="G2812" sqref="G2812:G3261"/>
+    <sheetView tabSelected="1" topLeftCell="A1403" workbookViewId="0">
+      <selection activeCell="G1936" sqref="G1936:G2024"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -85758,11 +85767,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -85773,7 +85782,7 @@
     <col min="5" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3260</v>
       </c>
@@ -85793,7 +85802,7 @@
         <v>3279</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -85810,7 +85819,7 @@
         <v>3268</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -85826,8 +85835,11 @@
       <c r="E3" t="s">
         <v>3271</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -85844,7 +85856,7 @@
         <v>3274</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -85860,8 +85872,11 @@
       <c r="E5" t="s">
         <v>3271</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -85869,7 +85884,7 @@
         <v>3278</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -85886,7 +85901,7 @@
         <v>3281</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -85903,7 +85918,7 @@
         <v>3281</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -85919,8 +85934,26 @@
       <c r="E9" t="s">
         <v>3281</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>1997</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1501</v>
+      </c>
+      <c r="I9" t="s">
+        <v>2023</v>
+      </c>
+      <c r="J9" t="s">
+        <v>3290</v>
+      </c>
+      <c r="K9" t="s">
+        <v>3291</v>
+      </c>
+      <c r="L9" t="s">
+        <v>3292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -85934,7 +85967,7 @@
         <v>3282</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -85948,7 +85981,7 @@
         <v>3284</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -85965,7 +85998,7 @@
         <v>3286</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -85980,6 +86013,9 @@
       </c>
       <c r="E13" t="s">
         <v>3289</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2860</v>
       </c>
     </row>
   </sheetData>

</xml_diff>